<commit_message>
merge savilerow into project
</commit_message>
<xml_diff>
--- a/comparison/mrcpsp/MMLIB50_STAIRCASE_2025-09-12-16-30-03.xlsx
+++ b/comparison/mrcpsp/MMLIB50_STAIRCASE_2025-09-12-16-30-03.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\MRCPSPTest\comparison\mrcpsp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\MRCPSPTest\comparison\mrcpsp\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104FE15E-250C-4EF7-BF4C-1C76BAEADFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17715"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MMLIB50_STAIRCASE_2025-09-12-16" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -1683,7 +1684,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2483,16 +2484,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K541"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2527,7 +2528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2562,7 +2563,7 @@
         <v>2.4199999999999998E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2597,7 +2598,7 @@
         <v>2.8600000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2632,7 +2633,7 @@
         <v>2.2899999999999999E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2667,7 +2668,7 @@
         <v>2.6700000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2702,7 +2703,7 @@
         <v>3.13E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2737,7 +2738,7 @@
         <v>4.4400000000000004E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -2772,7 +2773,7 @@
         <v>3.7200000000000002E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2807,7 +2808,7 @@
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -2842,7 +2843,7 @@
         <v>3.0799999999999998E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2877,7 +2878,7 @@
         <v>2.0300000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2912,7 +2913,7 @@
         <v>5.1700000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2947,7 +2948,7 @@
         <v>2.98E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2982,7 +2983,7 @@
         <v>6.13E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -3017,7 +3018,7 @@
         <v>3.0899999999999999E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -3052,7 +3053,7 @@
         <v>4.5700000000000003E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -3087,7 +3088,7 @@
         <v>2.4399999999999999E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -3122,7 +3123,7 @@
         <v>4.0800000000000003E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -3157,7 +3158,7 @@
         <v>4.0499999999999998E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -3192,7 +3193,7 @@
         <v>2.9099999999999998E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -3227,7 +3228,7 @@
         <v>4.3499999999999997E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -3262,7 +3263,7 @@
         <v>1.83E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -3297,7 +3298,7 @@
         <v>3.2499999999999999E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -3332,7 +3333,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -3367,7 +3368,7 @@
         <v>2.16E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -3402,7 +3403,7 @@
         <v>3.3700000000000002E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -3437,7 +3438,7 @@
         <v>5.2900000000000004E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -3472,7 +3473,7 @@
         <v>2.48E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -3507,7 +3508,7 @@
         <v>1.8799999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -3542,7 +3543,7 @@
         <v>2.0500000000000002E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -3577,7 +3578,7 @@
         <v>2.4499999999999999E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -3612,7 +3613,7 @@
         <v>3.8899999999999998E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -3647,7 +3648,7 @@
         <v>4.28E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -3682,7 +3683,7 @@
         <v>5.13E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -3717,7 +3718,7 @@
         <v>2.2399999999999998E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -3752,7 +3753,7 @@
         <v>2.8900000000000002E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -3787,7 +3788,7 @@
         <v>2.9499999999999999E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -3822,7 +3823,7 @@
         <v>2.0600000000000002E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -3857,7 +3858,7 @@
         <v>2.32E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -3892,7 +3893,7 @@
         <v>3.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -3927,7 +3928,7 @@
         <v>4.2300000000000003E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -3962,7 +3963,7 @@
         <v>3.9100000000000003E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -3997,7 +3998,7 @@
         <v>3.79E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -4032,7 +4033,7 @@
         <v>3.32E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -4067,7 +4068,7 @@
         <v>3.4499999999999999E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -4102,7 +4103,7 @@
         <v>4.2100000000000002E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -4137,7 +4138,7 @@
         <v>3.5400000000000002E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -4172,7 +4173,7 @@
         <v>1.91E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -4207,7 +4208,7 @@
         <v>3.14E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -4242,7 +4243,7 @@
         <v>3.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -4277,7 +4278,7 @@
         <v>2.2599999999999999E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -4312,7 +4313,7 @@
         <v>2.9299999999999999E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -4347,7 +4348,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -4382,7 +4383,7 @@
         <v>2.5500000000000002E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -4417,7 +4418,7 @@
         <v>5.8599999999999998E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -4452,7 +4453,7 @@
         <v>4.2399999999999998E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -4487,7 +4488,7 @@
         <v>2.3900000000000002E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>69</v>
       </c>
@@ -4522,7 +4523,7 @@
         <v>5.1700000000000001E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -4557,7 +4558,7 @@
         <v>4.2500000000000003E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>71</v>
       </c>
@@ -4592,7 +4593,7 @@
         <v>3.9899999999999996E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>72</v>
       </c>
@@ -4627,7 +4628,7 @@
         <v>3.3899999999999998E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>73</v>
       </c>
@@ -4662,7 +4663,7 @@
         <v>5.0400000000000002E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>74</v>
       </c>
@@ -4697,7 +4698,7 @@
         <v>5.8900000000000003E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>75</v>
       </c>
@@ -4732,7 +4733,7 @@
         <v>3.14E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>76</v>
       </c>
@@ -4767,7 +4768,7 @@
         <v>4.5900000000000003E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>77</v>
       </c>
@@ -4802,7 +4803,7 @@
         <v>1.82E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -4837,7 +4838,7 @@
         <v>2.7499999999999998E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -4872,7 +4873,7 @@
         <v>3.5500000000000002E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -4907,7 +4908,7 @@
         <v>3.4399999999999999E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>81</v>
       </c>
@@ -4942,7 +4943,7 @@
         <v>2.0300000000000001E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -4977,7 +4978,7 @@
         <v>4.79E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -5012,7 +5013,7 @@
         <v>4.7099999999999998E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>84</v>
       </c>
@@ -5047,7 +5048,7 @@
         <v>8.94E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -5082,7 +5083,7 @@
         <v>6.94E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>86</v>
       </c>
@@ -5117,7 +5118,7 @@
         <v>2.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>87</v>
       </c>
@@ -5152,7 +5153,7 @@
         <v>4.1000000000000003E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>88</v>
       </c>
@@ -5187,7 +5188,7 @@
         <v>4.0699999999999998E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>89</v>
       </c>
@@ -5222,7 +5223,7 @@
         <v>4.3099999999999996E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>90</v>
       </c>
@@ -5257,7 +5258,7 @@
         <v>3.6800000000000001E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>91</v>
       </c>
@@ -5292,7 +5293,7 @@
         <v>2.2300000000000002E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>92</v>
       </c>
@@ -5327,7 +5328,7 @@
         <v>2.7100000000000002E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>93</v>
       </c>
@@ -5362,7 +5363,7 @@
         <v>3.3700000000000002E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>94</v>
       </c>
@@ -5397,7 +5398,7 @@
         <v>5.77E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>95</v>
       </c>
@@ -5432,7 +5433,7 @@
         <v>2.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>96</v>
       </c>
@@ -5467,7 +5468,7 @@
         <v>3.0699999999999998E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>97</v>
       </c>
@@ -5502,7 +5503,7 @@
         <v>7.3899999999999999E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>98</v>
       </c>
@@ -5537,7 +5538,7 @@
         <v>5.7200000000000003E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>99</v>
       </c>
@@ -5572,7 +5573,7 @@
         <v>3.5300000000000002E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>100</v>
       </c>
@@ -5607,7 +5608,7 @@
         <v>4.7600000000000003E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>101</v>
       </c>
@@ -5642,7 +5643,7 @@
         <v>3.5500000000000002E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>102</v>
       </c>
@@ -5677,7 +5678,7 @@
         <v>3.5899999999999999E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>103</v>
       </c>
@@ -5712,7 +5713,7 @@
         <v>2.6900000000000001E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>104</v>
       </c>
@@ -5747,7 +5748,7 @@
         <v>4.7699999999999999E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>105</v>
       </c>
@@ -5782,7 +5783,7 @@
         <v>2.47E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>106</v>
       </c>
@@ -5817,7 +5818,7 @@
         <v>7.2199999999999999E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>107</v>
       </c>
@@ -5852,7 +5853,7 @@
         <v>3.8300000000000001E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>108</v>
       </c>
@@ -5887,7 +5888,7 @@
         <v>2.99E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>109</v>
       </c>
@@ -5922,7 +5923,7 @@
         <v>3.2599999999999999E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>110</v>
       </c>
@@ -5957,7 +5958,7 @@
         <v>3.48E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>111</v>
       </c>
@@ -5992,7 +5993,7 @@
         <v>4.1999999999999997E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>112</v>
       </c>
@@ -6027,7 +6028,7 @@
         <v>3.6700000000000001E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>113</v>
       </c>
@@ -6062,7 +6063,7 @@
         <v>3.4499999999999999E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>114</v>
       </c>
@@ -6097,7 +6098,7 @@
         <v>7.5300000000000002E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>115</v>
       </c>
@@ -6132,7 +6133,7 @@
         <v>2.5699999999999998E-3</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>116</v>
       </c>
@@ -6167,7 +6168,7 @@
         <v>1.91E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>117</v>
       </c>
@@ -6202,7 +6203,7 @@
         <v>3.98E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>118</v>
       </c>
@@ -6237,7 +6238,7 @@
         <v>2.2399999999999998E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>119</v>
       </c>
@@ -6272,7 +6273,7 @@
         <v>4.4200000000000003E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>120</v>
       </c>
@@ -6307,7 +6308,7 @@
         <v>2.64E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>121</v>
       </c>
@@ -6342,7 +6343,7 @@
         <v>2.8800000000000002E-3</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>122</v>
       </c>
@@ -6377,7 +6378,7 @@
         <v>3.1800000000000001E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>123</v>
       </c>
@@ -6412,7 +6413,7 @@
         <v>2.5600000000000002E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>124</v>
       </c>
@@ -6447,7 +6448,7 @@
         <v>3.7200000000000002E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>125</v>
       </c>
@@ -6482,7 +6483,7 @@
         <v>2.2499999999999998E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>126</v>
       </c>
@@ -6517,7 +6518,7 @@
         <v>6.0299999999999998E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>127</v>
       </c>
@@ -6552,7 +6553,7 @@
         <v>2.8600000000000001E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>128</v>
       </c>
@@ -6587,7 +6588,7 @@
         <v>3.65E-3</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>129</v>
       </c>
@@ -6622,7 +6623,7 @@
         <v>3.0500000000000002E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>130</v>
       </c>
@@ -6657,7 +6658,7 @@
         <v>2.2699999999999999E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>131</v>
       </c>
@@ -6692,7 +6693,7 @@
         <v>2.0699999999999998E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>132</v>
       </c>
@@ -6727,7 +6728,7 @@
         <v>7.8100000000000001E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>133</v>
       </c>
@@ -6762,7 +6763,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>134</v>
       </c>
@@ -6797,7 +6798,7 @@
         <v>5.4200000000000003E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>135</v>
       </c>
@@ -6832,7 +6833,7 @@
         <v>2.3700000000000001E-3</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>136</v>
       </c>
@@ -6867,7 +6868,7 @@
         <v>2.2399999999999998E-3</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>137</v>
       </c>
@@ -6902,7 +6903,7 @@
         <v>6.8500000000000002E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>138</v>
       </c>
@@ -6937,7 +6938,7 @@
         <v>6.0899999999999999E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>139</v>
       </c>
@@ -6972,7 +6973,7 @@
         <v>6.5700000000000003E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>140</v>
       </c>
@@ -7007,7 +7008,7 @@
         <v>6.1199999999999996E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>141</v>
       </c>
@@ -7042,7 +7043,7 @@
         <v>2.8700000000000002E-3</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>142</v>
       </c>
@@ -7077,7 +7078,7 @@
         <v>3.0200000000000001E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>143</v>
       </c>
@@ -7112,7 +7113,7 @@
         <v>8.0499999999999999E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>144</v>
       </c>
@@ -7147,7 +7148,7 @@
         <v>7.0099999999999997E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>145</v>
       </c>
@@ -7182,7 +7183,7 @@
         <v>4.2900000000000004E-3</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>146</v>
       </c>
@@ -7217,7 +7218,7 @@
         <v>2.3500000000000001E-3</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>147</v>
       </c>
@@ -7252,7 +7253,7 @@
         <v>2.63E-3</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>148</v>
       </c>
@@ -7287,7 +7288,7 @@
         <v>3.9300000000000003E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>149</v>
       </c>
@@ -7322,7 +7323,7 @@
         <v>4.9300000000000004E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>150</v>
       </c>
@@ -7357,7 +7358,7 @@
         <v>3.1900000000000001E-3</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>151</v>
       </c>
@@ -7392,7 +7393,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>152</v>
       </c>
@@ -7427,7 +7428,7 @@
         <v>3.46E-3</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>153</v>
       </c>
@@ -7462,7 +7463,7 @@
         <v>4.5100000000000001E-3</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>154</v>
       </c>
@@ -7497,7 +7498,7 @@
         <v>2.6900000000000001E-3</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>155</v>
       </c>
@@ -7532,7 +7533,7 @@
         <v>5.0699999999999999E-3</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>156</v>
       </c>
@@ -7567,7 +7568,7 @@
         <v>2.7899999999999999E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>157</v>
       </c>
@@ -7602,7 +7603,7 @@
         <v>6.4599999999999996E-3</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>158</v>
       </c>
@@ -7637,7 +7638,7 @@
         <v>1.89E-3</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>159</v>
       </c>
@@ -7672,7 +7673,7 @@
         <v>4.3299999999999996E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>160</v>
       </c>
@@ -7707,7 +7708,7 @@
         <v>2.8600000000000001E-3</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>161</v>
       </c>
@@ -7742,7 +7743,7 @@
         <v>5.45E-3</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>162</v>
       </c>
@@ -7777,7 +7778,7 @@
         <v>6.8300000000000001E-3</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>163</v>
       </c>
@@ -7812,7 +7813,7 @@
         <v>2.2799999999999999E-3</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>164</v>
       </c>
@@ -7847,7 +7848,7 @@
         <v>9.1699999999999993E-3</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>165</v>
       </c>
@@ -7882,7 +7883,7 @@
         <v>3.8700000000000002E-3</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>166</v>
       </c>
@@ -7917,7 +7918,7 @@
         <v>2.6199999999999999E-3</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>167</v>
       </c>
@@ -7952,7 +7953,7 @@
         <v>2.33E-3</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>168</v>
       </c>
@@ -7987,7 +7988,7 @@
         <v>2.8500000000000001E-3</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>169</v>
       </c>
@@ -8022,7 +8023,7 @@
         <v>5.8599999999999998E-3</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>170</v>
       </c>
@@ -8057,7 +8058,7 @@
         <v>2.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>171</v>
       </c>
@@ -8092,7 +8093,7 @@
         <v>4.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>172</v>
       </c>
@@ -8127,7 +8128,7 @@
         <v>5.28E-3</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>173</v>
       </c>
@@ -8162,7 +8163,7 @@
         <v>5.3699999999999998E-3</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>174</v>
       </c>
@@ -8197,7 +8198,7 @@
         <v>5.5199999999999997E-3</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>175</v>
       </c>
@@ -8232,7 +8233,7 @@
         <v>6.6899999999999998E-3</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>176</v>
       </c>
@@ -8267,7 +8268,7 @@
         <v>4.64E-3</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>177</v>
       </c>
@@ -8302,7 +8303,7 @@
         <v>2.63E-3</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>178</v>
       </c>
@@ -8337,7 +8338,7 @@
         <v>4.0499999999999998E-3</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>179</v>
       </c>
@@ -8372,7 +8373,7 @@
         <v>2.7899999999999999E-3</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>180</v>
       </c>
@@ -8407,7 +8408,7 @@
         <v>2.9299999999999999E-3</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>181</v>
       </c>
@@ -8442,7 +8443,7 @@
         <v>2.8700000000000002E-3</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>182</v>
       </c>
@@ -8477,7 +8478,7 @@
         <v>2.8900000000000002E-3</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>183</v>
       </c>
@@ -8512,7 +8513,7 @@
         <v>5.2100000000000002E-3</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>184</v>
       </c>
@@ -8547,7 +8548,7 @@
         <v>4.5500000000000002E-3</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>185</v>
       </c>
@@ -8582,7 +8583,7 @@
         <v>2.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>186</v>
       </c>
@@ -8617,7 +8618,7 @@
         <v>2.7599999999999999E-3</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>187</v>
       </c>
@@ -8652,7 +8653,7 @@
         <v>3.98E-3</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>188</v>
       </c>
@@ -8687,7 +8688,7 @@
         <v>2.3400000000000001E-3</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>189</v>
       </c>
@@ -8722,7 +8723,7 @@
         <v>4.0099999999999997E-3</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>190</v>
       </c>
@@ -8757,7 +8758,7 @@
         <v>5.8500000000000002E-3</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>191</v>
       </c>
@@ -8792,7 +8793,7 @@
         <v>4.4200000000000003E-3</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>192</v>
       </c>
@@ -8827,7 +8828,7 @@
         <v>2.2799999999999999E-3</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>193</v>
       </c>
@@ -8862,7 +8863,7 @@
         <v>2.9499999999999999E-3</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>194</v>
       </c>
@@ -8897,7 +8898,7 @@
         <v>2.5400000000000002E-3</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>195</v>
       </c>
@@ -8932,7 +8933,7 @@
         <v>4.7800000000000004E-3</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>196</v>
       </c>
@@ -8967,7 +8968,7 @@
         <v>4.28E-3</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>197</v>
       </c>
@@ -9002,7 +9003,7 @@
         <v>4.0699999999999998E-3</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>198</v>
       </c>
@@ -9037,7 +9038,7 @@
         <v>5.0400000000000002E-3</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>199</v>
       </c>
@@ -9072,7 +9073,7 @@
         <v>3.8600000000000001E-3</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>200</v>
       </c>
@@ -9107,7 +9108,7 @@
         <v>7.3299999999999997E-3</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>201</v>
       </c>
@@ -9142,7 +9143,7 @@
         <v>5.3800000000000002E-3</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>202</v>
       </c>
@@ -9177,7 +9178,7 @@
         <v>4.1999999999999997E-3</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>203</v>
       </c>
@@ -9212,7 +9213,7 @@
         <v>2.5100000000000001E-3</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>204</v>
       </c>
@@ -9247,7 +9248,7 @@
         <v>4.0200000000000001E-3</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>205</v>
       </c>
@@ -9282,7 +9283,7 @@
         <v>2.5699999999999998E-3</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>206</v>
       </c>
@@ -9317,7 +9318,7 @@
         <v>2.8300000000000001E-3</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>207</v>
       </c>
@@ -9352,7 +9353,7 @@
         <v>4.2599999999999999E-3</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>208</v>
       </c>
@@ -9387,7 +9388,7 @@
         <v>3.2599999999999999E-3</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>209</v>
       </c>
@@ -9422,7 +9423,7 @@
         <v>3.5100000000000001E-3</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>210</v>
       </c>
@@ -9457,7 +9458,7 @@
         <v>6.8799999999999998E-3</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>211</v>
       </c>
@@ -9492,7 +9493,7 @@
         <v>3.0799999999999998E-3</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>212</v>
       </c>
@@ -9527,7 +9528,7 @@
         <v>3.13E-3</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>213</v>
       </c>
@@ -9562,7 +9563,7 @@
         <v>6.3699999999999998E-3</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>214</v>
       </c>
@@ -9597,7 +9598,7 @@
         <v>3.1099999999999999E-3</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>215</v>
       </c>
@@ -9632,7 +9633,7 @@
         <v>5.0800000000000003E-3</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>216</v>
       </c>
@@ -9667,7 +9668,7 @@
         <v>4.6299999999999996E-3</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>217</v>
       </c>
@@ -9702,7 +9703,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>218</v>
       </c>
@@ -9737,7 +9738,7 @@
         <v>3.8600000000000001E-3</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>219</v>
       </c>
@@ -9772,7 +9773,7 @@
         <v>2.7399999999999998E-3</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>220</v>
       </c>
@@ -9807,7 +9808,7 @@
         <v>3.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>221</v>
       </c>
@@ -9842,7 +9843,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>222</v>
       </c>
@@ -9877,7 +9878,7 @@
         <v>3.31E-3</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>223</v>
       </c>
@@ -9912,7 +9913,7 @@
         <v>4.2199999999999998E-3</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>224</v>
       </c>
@@ -9947,7 +9948,7 @@
         <v>2.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>225</v>
       </c>
@@ -9982,7 +9983,7 @@
         <v>4.1799999999999997E-3</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>226</v>
       </c>
@@ -10017,7 +10018,7 @@
         <v>5.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>227</v>
       </c>
@@ -10052,7 +10053,7 @@
         <v>4.1099999999999999E-3</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>228</v>
       </c>
@@ -10087,7 +10088,7 @@
         <v>3.8300000000000001E-3</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>229</v>
       </c>
@@ -10122,7 +10123,7 @@
         <v>3.7399999999999998E-3</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>230</v>
       </c>
@@ -10157,7 +10158,7 @@
         <v>4.5900000000000003E-3</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>231</v>
       </c>
@@ -10192,7 +10193,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>232</v>
       </c>
@@ -10227,7 +10228,7 @@
         <v>2.3400000000000001E-3</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>233</v>
       </c>
@@ -10262,7 +10263,7 @@
         <v>3.2100000000000002E-3</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>234</v>
       </c>
@@ -10297,7 +10298,7 @@
         <v>7.7600000000000004E-3</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>235</v>
       </c>
@@ -10332,7 +10333,7 @@
         <v>2.3400000000000001E-3</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>236</v>
       </c>
@@ -10367,7 +10368,7 @@
         <v>7.7099999999999998E-3</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>237</v>
       </c>
@@ -10402,7 +10403,7 @@
         <v>3.82E-3</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>238</v>
       </c>
@@ -10437,7 +10438,7 @@
         <v>2.4599999999999999E-3</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>239</v>
       </c>
@@ -10472,7 +10473,7 @@
         <v>6.2399999999999999E-3</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>240</v>
       </c>
@@ -10507,7 +10508,7 @@
         <v>3.6099999999999999E-3</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>241</v>
       </c>
@@ -10542,7 +10543,7 @@
         <v>3.15E-3</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>242</v>
       </c>
@@ -10577,7 +10578,7 @@
         <v>2.3800000000000002E-3</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>243</v>
       </c>
@@ -10612,7 +10613,7 @@
         <v>2.0899999999999998E-3</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>244</v>
       </c>
@@ -10647,7 +10648,7 @@
         <v>5.1799999999999997E-3</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>245</v>
       </c>
@@ -10682,7 +10683,7 @@
         <v>2.8500000000000001E-3</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>246</v>
       </c>
@@ -10717,7 +10718,7 @@
         <v>3.1099999999999999E-3</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>247</v>
       </c>
@@ -10752,7 +10753,7 @@
         <v>6.7200000000000003E-3</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>248</v>
       </c>
@@ -10787,7 +10788,7 @@
         <v>2.7499999999999998E-3</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>249</v>
       </c>
@@ -10822,7 +10823,7 @@
         <v>3.3500000000000001E-3</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>250</v>
       </c>
@@ -10857,7 +10858,7 @@
         <v>2.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>251</v>
       </c>
@@ -10892,7 +10893,7 @@
         <v>3.48E-3</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>252</v>
       </c>
@@ -10927,7 +10928,7 @@
         <v>7.8200000000000006E-3</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>253</v>
       </c>
@@ -10962,7 +10963,7 @@
         <v>3.5899999999999999E-3</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>254</v>
       </c>
@@ -10997,7 +10998,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>255</v>
       </c>
@@ -11032,7 +11033,7 @@
         <v>5.0699999999999999E-3</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>256</v>
       </c>
@@ -11067,7 +11068,7 @@
         <v>4.1000000000000003E-3</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>257</v>
       </c>
@@ -11102,7 +11103,7 @@
         <v>6.0099999999999997E-3</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>258</v>
       </c>
@@ -11137,7 +11138,7 @@
         <v>2.2399999999999998E-3</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>259</v>
       </c>
@@ -11172,7 +11173,7 @@
         <v>3.62E-3</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>260</v>
       </c>
@@ -11207,7 +11208,7 @@
         <v>4.8799999999999998E-3</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>261</v>
       </c>
@@ -11242,7 +11243,7 @@
         <v>5.2100000000000002E-3</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>262</v>
       </c>
@@ -11277,7 +11278,7 @@
         <v>3.6800000000000001E-3</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>263</v>
       </c>
@@ -11312,7 +11313,7 @@
         <v>4.2100000000000002E-3</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>264</v>
       </c>
@@ -11347,7 +11348,7 @@
         <v>2.63E-3</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>265</v>
       </c>
@@ -11382,7 +11383,7 @@
         <v>4.6499999999999996E-3</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>266</v>
       </c>
@@ -11417,7 +11418,7 @@
         <v>4.8300000000000001E-3</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>267</v>
       </c>
@@ -11452,7 +11453,7 @@
         <v>4.81E-3</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>268</v>
       </c>
@@ -11487,7 +11488,7 @@
         <v>5.6499999999999996E-3</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>269</v>
       </c>
@@ -11522,7 +11523,7 @@
         <v>7.0299999999999998E-3</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>270</v>
       </c>
@@ -11557,7 +11558,7 @@
         <v>3.2200000000000002E-3</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>271</v>
       </c>
@@ -11592,7 +11593,7 @@
         <v>4.1900000000000001E-3</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>272</v>
       </c>
@@ -11627,7 +11628,7 @@
         <v>3.0100000000000001E-3</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>273</v>
       </c>
@@ -11662,7 +11663,7 @@
         <v>3.6600000000000001E-3</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>274</v>
       </c>
@@ -11697,7 +11698,7 @@
         <v>3.3700000000000002E-3</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>275</v>
       </c>
@@ -11732,7 +11733,7 @@
         <v>6.0400000000000002E-3</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>276</v>
       </c>
@@ -11767,7 +11768,7 @@
         <v>2.2399999999999998E-3</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>277</v>
       </c>
@@ -11802,7 +11803,7 @@
         <v>8.8299999999999993E-3</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>278</v>
       </c>
@@ -11837,7 +11838,7 @@
         <v>4.6600000000000001E-3</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>279</v>
       </c>
@@ -11872,7 +11873,7 @@
         <v>4.1099999999999999E-3</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>280</v>
       </c>
@@ -11907,7 +11908,7 @@
         <v>5.5700000000000003E-3</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>281</v>
       </c>
@@ -11942,7 +11943,7 @@
         <v>2.98E-3</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>282</v>
       </c>
@@ -11977,7 +11978,7 @@
         <v>8.5800000000000008E-3</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>283</v>
       </c>
@@ -12012,7 +12013,7 @@
         <v>2.8700000000000002E-3</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>284</v>
       </c>
@@ -12047,7 +12048,7 @@
         <v>3.65E-3</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>285</v>
       </c>
@@ -12082,7 +12083,7 @@
         <v>3.0200000000000001E-3</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>286</v>
       </c>
@@ -12117,7 +12118,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>287</v>
       </c>
@@ -12152,7 +12153,7 @@
         <v>2.3E-3</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>288</v>
       </c>
@@ -12187,7 +12188,7 @@
         <v>6.45E-3</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>289</v>
       </c>
@@ -12222,7 +12223,7 @@
         <v>5.2900000000000004E-3</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>290</v>
       </c>
@@ -12257,7 +12258,7 @@
         <v>5.2599999999999999E-3</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>291</v>
       </c>
@@ -12292,7 +12293,7 @@
         <v>2.5500000000000002E-3</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>292</v>
       </c>
@@ -12327,7 +12328,7 @@
         <v>6.4799999999999996E-3</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>293</v>
       </c>
@@ -12362,7 +12363,7 @@
         <v>4.0400000000000002E-3</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>294</v>
       </c>
@@ -12397,7 +12398,7 @@
         <v>3.9899999999999996E-3</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>295</v>
       </c>
@@ -12432,7 +12433,7 @@
         <v>6.0899999999999999E-3</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>296</v>
       </c>
@@ -12467,7 +12468,7 @@
         <v>5.4799999999999996E-3</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>297</v>
       </c>
@@ -12502,7 +12503,7 @@
         <v>2.8800000000000002E-3</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>298</v>
       </c>
@@ -12537,7 +12538,7 @@
         <v>5.9899999999999997E-3</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>299</v>
       </c>
@@ -12572,7 +12573,7 @@
         <v>3.0100000000000001E-3</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>300</v>
       </c>
@@ -12607,7 +12608,7 @@
         <v>2.48E-3</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>301</v>
       </c>
@@ -12642,7 +12643,7 @@
         <v>2.8700000000000002E-3</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>302</v>
       </c>
@@ -12677,7 +12678,7 @@
         <v>5.4599999999999996E-3</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>303</v>
       </c>
@@ -12712,7 +12713,7 @@
         <v>8.4399999999999996E-3</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>304</v>
       </c>
@@ -12747,7 +12748,7 @@
         <v>5.4299999999999999E-3</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>305</v>
       </c>
@@ -12782,7 +12783,7 @@
         <v>5.9100000000000003E-3</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>306</v>
       </c>
@@ -12817,7 +12818,7 @@
         <v>4.1399999999999996E-3</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>307</v>
       </c>
@@ -12852,7 +12853,7 @@
         <v>4.3400000000000001E-3</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>308</v>
       </c>
@@ -12887,7 +12888,7 @@
         <v>6.45E-3</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>309</v>
       </c>
@@ -12922,7 +12923,7 @@
         <v>3.1900000000000001E-3</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>310</v>
       </c>
@@ -12957,7 +12958,7 @@
         <v>2.2799999999999999E-3</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>311</v>
       </c>
@@ -12992,7 +12993,7 @@
         <v>2.9499999999999999E-3</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>312</v>
       </c>
@@ -13027,7 +13028,7 @@
         <v>6.3699999999999998E-3</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>313</v>
       </c>
@@ -13062,7 +13063,7 @@
         <v>6.8399999999999997E-3</v>
       </c>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>314</v>
       </c>
@@ -13097,7 +13098,7 @@
         <v>6.7400000000000003E-3</v>
       </c>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>315</v>
       </c>
@@ -13132,7 +13133,7 @@
         <v>4.3400000000000001E-3</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>316</v>
       </c>
@@ -13167,7 +13168,7 @@
         <v>6.4700000000000001E-3</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>317</v>
       </c>
@@ -13202,7 +13203,7 @@
         <v>4.0600000000000002E-3</v>
       </c>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>318</v>
       </c>
@@ -13237,7 +13238,7 @@
         <v>4.3200000000000001E-3</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>319</v>
       </c>
@@ -13272,7 +13273,7 @@
         <v>2.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>320</v>
       </c>
@@ -13307,7 +13308,7 @@
         <v>5.28E-3</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>321</v>
       </c>
@@ -13342,7 +13343,7 @@
         <v>5.96E-3</v>
       </c>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>322</v>
       </c>
@@ -13377,7 +13378,7 @@
         <v>2.5200000000000001E-3</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>323</v>
       </c>
@@ -13412,7 +13413,7 @@
         <v>2.8900000000000002E-3</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>324</v>
       </c>
@@ -13447,7 +13448,7 @@
         <v>7.43E-3</v>
       </c>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>325</v>
       </c>
@@ -13482,7 +13483,7 @@
         <v>4.8700000000000002E-3</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>326</v>
       </c>
@@ -13517,7 +13518,7 @@
         <v>5.7299999999999999E-3</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>327</v>
       </c>
@@ -13552,7 +13553,7 @@
         <v>3.7499999999999999E-3</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>328</v>
       </c>
@@ -13587,7 +13588,7 @@
         <v>3.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>329</v>
       </c>
@@ -13622,7 +13623,7 @@
         <v>4.6100000000000004E-3</v>
       </c>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>330</v>
       </c>
@@ -13657,7 +13658,7 @@
         <v>3.6900000000000001E-3</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>331</v>
       </c>
@@ -13692,7 +13693,7 @@
         <v>2.7200000000000002E-3</v>
       </c>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>332</v>
       </c>
@@ -13727,7 +13728,7 @@
         <v>5.9800000000000001E-3</v>
       </c>
     </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>333</v>
       </c>
@@ -13762,7 +13763,7 @@
         <v>3.2599999999999999E-3</v>
       </c>
     </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>334</v>
       </c>
@@ -13797,7 +13798,7 @@
         <v>3.0599999999999998E-3</v>
       </c>
     </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>335</v>
       </c>
@@ -13832,7 +13833,7 @@
         <v>4.7099999999999998E-3</v>
       </c>
     </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>336</v>
       </c>
@@ -13867,7 +13868,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>337</v>
       </c>
@@ -13902,7 +13903,7 @@
         <v>4.4400000000000004E-3</v>
       </c>
     </row>
-    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>338</v>
       </c>
@@ -13937,7 +13938,7 @@
         <v>3.3700000000000002E-3</v>
       </c>
     </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>339</v>
       </c>
@@ -13972,7 +13973,7 @@
         <v>2.8700000000000002E-3</v>
       </c>
     </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>340</v>
       </c>
@@ -14007,7 +14008,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>341</v>
       </c>
@@ -14042,7 +14043,7 @@
         <v>7.28E-3</v>
       </c>
     </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>342</v>
       </c>
@@ -14077,7 +14078,7 @@
         <v>5.4200000000000003E-3</v>
       </c>
     </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>343</v>
       </c>
@@ -14112,7 +14113,7 @@
         <v>2.7399999999999998E-3</v>
       </c>
     </row>
-    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>344</v>
       </c>
@@ -14147,7 +14148,7 @@
         <v>4.1999999999999997E-3</v>
       </c>
     </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>345</v>
       </c>
@@ -14182,7 +14183,7 @@
         <v>4.4900000000000001E-3</v>
       </c>
     </row>
-    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>346</v>
       </c>
@@ -14217,7 +14218,7 @@
         <v>5.5300000000000002E-3</v>
       </c>
     </row>
-    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>347</v>
       </c>
@@ -14252,7 +14253,7 @@
         <v>2.7200000000000002E-3</v>
       </c>
     </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>348</v>
       </c>
@@ -14287,7 +14288,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>349</v>
       </c>
@@ -14322,7 +14323,7 @@
         <v>4.6899999999999997E-3</v>
       </c>
     </row>
-    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>350</v>
       </c>
@@ -14357,7 +14358,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>351</v>
       </c>
@@ -14392,7 +14393,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>352</v>
       </c>
@@ -14427,7 +14428,7 @@
         <v>8.9700000000000005E-3</v>
       </c>
     </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>353</v>
       </c>
@@ -14462,7 +14463,7 @@
         <v>2.66E-3</v>
       </c>
     </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>354</v>
       </c>
@@ -14497,7 +14498,7 @@
         <v>2.0500000000000002E-3</v>
       </c>
     </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>355</v>
       </c>
@@ -14532,7 +14533,7 @@
         <v>6.4799999999999996E-3</v>
       </c>
     </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>356</v>
       </c>
@@ -14567,7 +14568,7 @@
         <v>6.45E-3</v>
       </c>
     </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>357</v>
       </c>
@@ -14602,7 +14603,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
     </row>
-    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>358</v>
       </c>
@@ -14637,7 +14638,7 @@
         <v>6.2399999999999999E-3</v>
       </c>
     </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>359</v>
       </c>
@@ -14672,7 +14673,7 @@
         <v>6.4799999999999996E-3</v>
       </c>
     </row>
-    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>360</v>
       </c>
@@ -14707,7 +14708,7 @@
         <v>3.6099999999999999E-3</v>
       </c>
     </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>361</v>
       </c>
@@ -14742,7 +14743,7 @@
         <v>3.5100000000000001E-3</v>
       </c>
     </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>362</v>
       </c>
@@ -14777,7 +14778,7 @@
         <v>3.0300000000000001E-3</v>
       </c>
     </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>363</v>
       </c>
@@ -14812,7 +14813,7 @@
         <v>3.49E-3</v>
       </c>
     </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>364</v>
       </c>
@@ -14847,7 +14848,7 @@
         <v>7.6600000000000001E-3</v>
       </c>
     </row>
-    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>365</v>
       </c>
@@ -14882,7 +14883,7 @@
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>366</v>
       </c>
@@ -14917,7 +14918,7 @@
         <v>6.8300000000000001E-3</v>
       </c>
     </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>367</v>
       </c>
@@ -14952,7 +14953,7 @@
         <v>2.5300000000000001E-3</v>
       </c>
     </row>
-    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>368</v>
       </c>
@@ -14987,7 +14988,7 @@
         <v>4.81E-3</v>
       </c>
     </row>
-    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>369</v>
       </c>
@@ -15022,7 +15023,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>370</v>
       </c>
@@ -15057,7 +15058,7 @@
         <v>2.9099999999999998E-3</v>
       </c>
     </row>
-    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>371</v>
       </c>
@@ -15092,7 +15093,7 @@
         <v>3.1199999999999999E-3</v>
       </c>
     </row>
-    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>372</v>
       </c>
@@ -15127,7 +15128,7 @@
         <v>4.6699999999999997E-3</v>
       </c>
     </row>
-    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>373</v>
       </c>
@@ -15162,7 +15163,7 @@
         <v>4.2900000000000004E-3</v>
       </c>
     </row>
-    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>374</v>
       </c>
@@ -15197,7 +15198,7 @@
         <v>4.81E-3</v>
       </c>
     </row>
-    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>375</v>
       </c>
@@ -15232,7 +15233,7 @@
         <v>5.1700000000000001E-3</v>
       </c>
     </row>
-    <row r="365" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>376</v>
       </c>
@@ -15267,7 +15268,7 @@
         <v>6.0800000000000003E-3</v>
       </c>
     </row>
-    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>377</v>
       </c>
@@ -15302,7 +15303,7 @@
         <v>3.31E-3</v>
       </c>
     </row>
-    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>378</v>
       </c>
@@ -15337,7 +15338,7 @@
         <v>3.6600000000000001E-3</v>
       </c>
     </row>
-    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>379</v>
       </c>
@@ -15372,7 +15373,7 @@
         <v>3.48E-3</v>
       </c>
     </row>
-    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>380</v>
       </c>
@@ -15407,7 +15408,7 @@
         <v>2.8600000000000001E-3</v>
       </c>
     </row>
-    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>381</v>
       </c>
@@ -15442,7 +15443,7 @@
         <v>6.3200000000000001E-3</v>
       </c>
     </row>
-    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>382</v>
       </c>
@@ -15477,7 +15478,7 @@
         <v>2.0300000000000001E-3</v>
       </c>
     </row>
-    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>383</v>
       </c>
@@ -15512,7 +15513,7 @@
         <v>4.8500000000000001E-3</v>
       </c>
     </row>
-    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>384</v>
       </c>
@@ -15547,7 +15548,7 @@
         <v>3.1700000000000001E-3</v>
       </c>
     </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>385</v>
       </c>
@@ -15582,7 +15583,7 @@
         <v>2.7599999999999999E-3</v>
       </c>
     </row>
-    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>386</v>
       </c>
@@ -15617,7 +15618,7 @@
         <v>3.4499999999999999E-3</v>
       </c>
     </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>387</v>
       </c>
@@ -15652,7 +15653,7 @@
         <v>2.9399999999999999E-3</v>
       </c>
     </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>388</v>
       </c>
@@ -15687,7 +15688,7 @@
         <v>4.5100000000000001E-3</v>
       </c>
     </row>
-    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>389</v>
       </c>
@@ -15722,7 +15723,7 @@
         <v>2.7100000000000002E-3</v>
       </c>
     </row>
-    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>390</v>
       </c>
@@ -15757,7 +15758,7 @@
         <v>2.47E-3</v>
       </c>
     </row>
-    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>391</v>
       </c>
@@ -15792,7 +15793,7 @@
         <v>3.0699999999999998E-3</v>
       </c>
     </row>
-    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>392</v>
       </c>
@@ -15827,7 +15828,7 @@
         <v>2.0799999999999998E-3</v>
       </c>
     </row>
-    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>393</v>
       </c>
@@ -15862,7 +15863,7 @@
         <v>7.45E-3</v>
       </c>
     </row>
-    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>394</v>
       </c>
@@ -15897,7 +15898,7 @@
         <v>4.3899999999999998E-3</v>
       </c>
     </row>
-    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>395</v>
       </c>
@@ -15932,7 +15933,7 @@
         <v>3.8899999999999998E-3</v>
       </c>
     </row>
-    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>396</v>
       </c>
@@ -15967,7 +15968,7 @@
         <v>4.2300000000000003E-3</v>
       </c>
     </row>
-    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
         <v>397</v>
       </c>
@@ -16002,7 +16003,7 @@
         <v>3.2000000000000002E-3</v>
       </c>
     </row>
-    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
         <v>398</v>
       </c>
@@ -16037,7 +16038,7 @@
         <v>5.2700000000000004E-3</v>
       </c>
     </row>
-    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
         <v>399</v>
       </c>
@@ -16072,7 +16073,7 @@
         <v>4.6299999999999996E-3</v>
       </c>
     </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>400</v>
       </c>
@@ -16107,7 +16108,7 @@
         <v>4.0499999999999998E-3</v>
       </c>
     </row>
-    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
         <v>401</v>
       </c>
@@ -16142,7 +16143,7 @@
         <v>5.0499999999999998E-3</v>
       </c>
     </row>
-    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
         <v>402</v>
       </c>
@@ -16177,7 +16178,7 @@
         <v>3.5599999999999998E-3</v>
       </c>
     </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>403</v>
       </c>
@@ -16212,7 +16213,7 @@
         <v>2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>404</v>
       </c>
@@ -16247,7 +16248,7 @@
         <v>6.11E-3</v>
       </c>
     </row>
-    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>405</v>
       </c>
@@ -16282,7 +16283,7 @@
         <v>4.81E-3</v>
       </c>
     </row>
-    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>406</v>
       </c>
@@ -16317,7 +16318,7 @@
         <v>5.3899999999999998E-3</v>
       </c>
     </row>
-    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>407</v>
       </c>
@@ -16352,7 +16353,7 @@
         <v>4.1000000000000003E-3</v>
       </c>
     </row>
-    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>408</v>
       </c>
@@ -16387,7 +16388,7 @@
         <v>4.4900000000000001E-3</v>
       </c>
     </row>
-    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>409</v>
       </c>
@@ -16422,7 +16423,7 @@
         <v>2.0899999999999998E-3</v>
       </c>
     </row>
-    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>410</v>
       </c>
@@ -16457,7 +16458,7 @@
         <v>5.6899999999999997E-3</v>
       </c>
     </row>
-    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>411</v>
       </c>
@@ -16492,7 +16493,7 @@
         <v>4.4799999999999996E-3</v>
       </c>
     </row>
-    <row r="401" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>412</v>
       </c>
@@ -16527,7 +16528,7 @@
         <v>3.1900000000000001E-3</v>
       </c>
     </row>
-    <row r="402" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>413</v>
       </c>
@@ -16562,7 +16563,7 @@
         <v>5.7099999999999998E-3</v>
       </c>
     </row>
-    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>414</v>
       </c>
@@ -16597,7 +16598,7 @@
         <v>4.5799999999999999E-3</v>
       </c>
     </row>
-    <row r="404" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>415</v>
       </c>
@@ -16632,7 +16633,7 @@
         <v>4.4400000000000004E-3</v>
       </c>
     </row>
-    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>416</v>
       </c>
@@ -16667,7 +16668,7 @@
         <v>1.8500000000000001E-3</v>
       </c>
     </row>
-    <row r="406" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>417</v>
       </c>
@@ -16702,7 +16703,7 @@
         <v>3.1800000000000001E-3</v>
       </c>
     </row>
-    <row r="407" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>418</v>
       </c>
@@ -16737,7 +16738,7 @@
         <v>3.9699999999999996E-3</v>
       </c>
     </row>
-    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>419</v>
       </c>
@@ -16772,7 +16773,7 @@
         <v>2.4099999999999998E-3</v>
       </c>
     </row>
-    <row r="409" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>420</v>
       </c>
@@ -16807,7 +16808,7 @@
         <v>4.3800000000000002E-3</v>
       </c>
     </row>
-    <row r="410" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>421</v>
       </c>
@@ -16842,7 +16843,7 @@
         <v>6.2500000000000003E-3</v>
       </c>
     </row>
-    <row r="411" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>422</v>
       </c>
@@ -16877,7 +16878,7 @@
         <v>2.82E-3</v>
       </c>
     </row>
-    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>423</v>
       </c>
@@ -16912,7 +16913,7 @@
         <v>2.7499999999999998E-3</v>
       </c>
     </row>
-    <row r="413" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
         <v>424</v>
       </c>
@@ -16947,7 +16948,7 @@
         <v>5.5300000000000002E-3</v>
       </c>
     </row>
-    <row r="414" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
         <v>425</v>
       </c>
@@ -16982,7 +16983,7 @@
         <v>2.65E-3</v>
       </c>
     </row>
-    <row r="415" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
         <v>426</v>
       </c>
@@ -17017,7 +17018,7 @@
         <v>4.1599999999999996E-3</v>
       </c>
     </row>
-    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
         <v>427</v>
       </c>
@@ -17052,7 +17053,7 @@
         <v>3.63E-3</v>
       </c>
     </row>
-    <row r="417" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>428</v>
       </c>
@@ -17087,7 +17088,7 @@
         <v>3.46E-3</v>
       </c>
     </row>
-    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>429</v>
       </c>
@@ -17122,7 +17123,7 @@
         <v>6.0099999999999997E-3</v>
       </c>
     </row>
-    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
         <v>430</v>
       </c>
@@ -17157,7 +17158,7 @@
         <v>3.7699999999999999E-3</v>
       </c>
     </row>
-    <row r="420" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
         <v>431</v>
       </c>
@@ -17192,7 +17193,7 @@
         <v>5.9899999999999997E-3</v>
       </c>
     </row>
-    <row r="421" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
         <v>432</v>
       </c>
@@ -17227,7 +17228,7 @@
         <v>2.32E-3</v>
       </c>
     </row>
-    <row r="422" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
         <v>433</v>
       </c>
@@ -17262,7 +17263,7 @@
         <v>2.5300000000000001E-3</v>
       </c>
     </row>
-    <row r="423" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
         <v>434</v>
       </c>
@@ -17297,7 +17298,7 @@
         <v>4.8700000000000002E-3</v>
       </c>
     </row>
-    <row r="424" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
         <v>435</v>
       </c>
@@ -17332,7 +17333,7 @@
         <v>4.79E-3</v>
       </c>
     </row>
-    <row r="425" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
         <v>436</v>
       </c>
@@ -17367,7 +17368,7 @@
         <v>2.65E-3</v>
       </c>
     </row>
-    <row r="426" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
         <v>437</v>
       </c>
@@ -17402,7 +17403,7 @@
         <v>3.0100000000000001E-3</v>
       </c>
     </row>
-    <row r="427" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
         <v>438</v>
       </c>
@@ -17437,7 +17438,7 @@
         <v>3.3400000000000001E-3</v>
       </c>
     </row>
-    <row r="428" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
         <v>439</v>
       </c>
@@ -17472,7 +17473,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="429" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
         <v>440</v>
       </c>
@@ -17507,7 +17508,7 @@
         <v>5.0600000000000003E-3</v>
       </c>
     </row>
-    <row r="430" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
         <v>441</v>
       </c>
@@ -17542,7 +17543,7 @@
         <v>4.7699999999999999E-3</v>
       </c>
     </row>
-    <row r="431" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
         <v>442</v>
       </c>
@@ -17577,7 +17578,7 @@
         <v>3.5200000000000001E-3</v>
       </c>
     </row>
-    <row r="432" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A432" t="s">
         <v>443</v>
       </c>
@@ -17612,7 +17613,7 @@
         <v>2.3800000000000002E-3</v>
       </c>
     </row>
-    <row r="433" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
         <v>444</v>
       </c>
@@ -17647,7 +17648,7 @@
         <v>2.2200000000000002E-3</v>
       </c>
     </row>
-    <row r="434" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
         <v>445</v>
       </c>
@@ -17682,7 +17683,7 @@
         <v>3.3899999999999998E-3</v>
       </c>
     </row>
-    <row r="435" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
         <v>446</v>
       </c>
@@ -17717,7 +17718,7 @@
         <v>5.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="436" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
         <v>447</v>
       </c>
@@ -17752,7 +17753,7 @@
         <v>2.7200000000000002E-3</v>
       </c>
     </row>
-    <row r="437" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
         <v>448</v>
       </c>
@@ -17787,7 +17788,7 @@
         <v>5.1700000000000001E-3</v>
       </c>
     </row>
-    <row r="438" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A438" t="s">
         <v>449</v>
       </c>
@@ -17822,7 +17823,7 @@
         <v>3.8899999999999998E-3</v>
       </c>
     </row>
-    <row r="439" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
         <v>450</v>
       </c>
@@ -17857,7 +17858,7 @@
         <v>6.43E-3</v>
       </c>
     </row>
-    <row r="440" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
         <v>451</v>
       </c>
@@ -17892,7 +17893,7 @@
         <v>3.2799999999999999E-3</v>
       </c>
     </row>
-    <row r="441" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
         <v>452</v>
       </c>
@@ -17927,7 +17928,7 @@
         <v>3.64E-3</v>
       </c>
     </row>
-    <row r="442" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A442" t="s">
         <v>453</v>
       </c>
@@ -17962,7 +17963,7 @@
         <v>2.3500000000000001E-3</v>
       </c>
     </row>
-    <row r="443" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
         <v>454</v>
       </c>
@@ -17997,7 +17998,7 @@
         <v>3.1099999999999999E-3</v>
       </c>
     </row>
-    <row r="444" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A444" t="s">
         <v>455</v>
       </c>
@@ -18032,7 +18033,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="445" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A445" t="s">
         <v>456</v>
       </c>
@@ -18067,7 +18068,7 @@
         <v>2.98E-3</v>
       </c>
     </row>
-    <row r="446" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
         <v>457</v>
       </c>
@@ -18102,7 +18103,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="447" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
         <v>458</v>
       </c>
@@ -18137,7 +18138,7 @@
         <v>4.2300000000000003E-3</v>
       </c>
     </row>
-    <row r="448" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A448" t="s">
         <v>459</v>
       </c>
@@ -18172,7 +18173,7 @@
         <v>6.0400000000000002E-3</v>
       </c>
     </row>
-    <row r="449" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A449" t="s">
         <v>460</v>
       </c>
@@ -18207,7 +18208,7 @@
         <v>5.0400000000000002E-3</v>
       </c>
     </row>
-    <row r="450" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A450" t="s">
         <v>461</v>
       </c>
@@ -18242,7 +18243,7 @@
         <v>6.3800000000000003E-3</v>
       </c>
     </row>
-    <row r="451" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
         <v>462</v>
       </c>
@@ -18277,7 +18278,7 @@
         <v>3.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="452" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A452" t="s">
         <v>463</v>
       </c>
@@ -18312,7 +18313,7 @@
         <v>3.82E-3</v>
       </c>
     </row>
-    <row r="453" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A453" t="s">
         <v>464</v>
       </c>
@@ -18347,7 +18348,7 @@
         <v>4.3299999999999996E-3</v>
       </c>
     </row>
-    <row r="454" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A454" t="s">
         <v>465</v>
       </c>
@@ -18382,7 +18383,7 @@
         <v>3.0300000000000001E-3</v>
       </c>
     </row>
-    <row r="455" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A455" t="s">
         <v>466</v>
       </c>
@@ -18417,7 +18418,7 @@
         <v>2.9399999999999999E-3</v>
       </c>
     </row>
-    <row r="456" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A456" t="s">
         <v>467</v>
       </c>
@@ -18452,7 +18453,7 @@
         <v>4.0099999999999997E-3</v>
       </c>
     </row>
-    <row r="457" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A457" t="s">
         <v>468</v>
       </c>
@@ -18487,7 +18488,7 @@
         <v>5.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="458" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A458" t="s">
         <v>469</v>
       </c>
@@ -18522,7 +18523,7 @@
         <v>3.3800000000000002E-3</v>
       </c>
     </row>
-    <row r="459" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A459" t="s">
         <v>470</v>
       </c>
@@ -18557,7 +18558,7 @@
         <v>2.5500000000000002E-3</v>
       </c>
     </row>
-    <row r="460" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
         <v>471</v>
       </c>
@@ -18592,7 +18593,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="461" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
         <v>472</v>
       </c>
@@ -18627,7 +18628,7 @@
         <v>4.7400000000000003E-3</v>
       </c>
     </row>
-    <row r="462" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A462" t="s">
         <v>473</v>
       </c>
@@ -18662,7 +18663,7 @@
         <v>2.6099999999999999E-3</v>
       </c>
     </row>
-    <row r="463" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
         <v>474</v>
       </c>
@@ -18697,7 +18698,7 @@
         <v>2.8300000000000001E-3</v>
       </c>
     </row>
-    <row r="464" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
         <v>475</v>
       </c>
@@ -18732,7 +18733,7 @@
         <v>7.11E-3</v>
       </c>
     </row>
-    <row r="465" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
         <v>476</v>
       </c>
@@ -18767,7 +18768,7 @@
         <v>3.3700000000000002E-3</v>
       </c>
     </row>
-    <row r="466" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
         <v>477</v>
       </c>
@@ -18802,7 +18803,7 @@
         <v>3.4499999999999999E-3</v>
       </c>
     </row>
-    <row r="467" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
         <v>478</v>
       </c>
@@ -18837,7 +18838,7 @@
         <v>7.7799999999999996E-3</v>
       </c>
     </row>
-    <row r="468" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A468" t="s">
         <v>479</v>
       </c>
@@ -18872,7 +18873,7 @@
         <v>6.0800000000000003E-3</v>
       </c>
     </row>
-    <row r="469" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A469" t="s">
         <v>480</v>
       </c>
@@ -18907,7 +18908,7 @@
         <v>5.2700000000000004E-3</v>
       </c>
     </row>
-    <row r="470" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A470" t="s">
         <v>481</v>
       </c>
@@ -18942,7 +18943,7 @@
         <v>4.5900000000000003E-3</v>
       </c>
     </row>
-    <row r="471" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A471" t="s">
         <v>482</v>
       </c>
@@ -18977,7 +18978,7 @@
         <v>3.4199999999999999E-3</v>
       </c>
     </row>
-    <row r="472" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A472" t="s">
         <v>483</v>
       </c>
@@ -19012,7 +19013,7 @@
         <v>4.6600000000000001E-3</v>
       </c>
     </row>
-    <row r="473" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A473" t="s">
         <v>484</v>
       </c>
@@ -19047,7 +19048,7 @@
         <v>2.8900000000000002E-3</v>
       </c>
     </row>
-    <row r="474" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A474" t="s">
         <v>485</v>
       </c>
@@ -19082,7 +19083,7 @@
         <v>2.3E-3</v>
       </c>
     </row>
-    <row r="475" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A475" t="s">
         <v>486</v>
       </c>
@@ -19117,7 +19118,7 @@
         <v>3.63E-3</v>
       </c>
     </row>
-    <row r="476" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A476" t="s">
         <v>487</v>
       </c>
@@ -19152,7 +19153,7 @@
         <v>5.7800000000000004E-3</v>
       </c>
     </row>
-    <row r="477" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A477" t="s">
         <v>488</v>
       </c>
@@ -19187,7 +19188,7 @@
         <v>3.5200000000000001E-3</v>
       </c>
     </row>
-    <row r="478" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A478" t="s">
         <v>489</v>
       </c>
@@ -19222,7 +19223,7 @@
         <v>3.0300000000000001E-3</v>
       </c>
     </row>
-    <row r="479" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A479" t="s">
         <v>490</v>
       </c>
@@ -19257,7 +19258,7 @@
         <v>4.6299999999999996E-3</v>
       </c>
     </row>
-    <row r="480" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A480" t="s">
         <v>491</v>
       </c>
@@ -19292,7 +19293,7 @@
         <v>2.7599999999999999E-3</v>
       </c>
     </row>
-    <row r="481" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
         <v>492</v>
       </c>
@@ -19327,7 +19328,7 @@
         <v>4.8300000000000001E-3</v>
       </c>
     </row>
-    <row r="482" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A482" t="s">
         <v>493</v>
       </c>
@@ -19362,7 +19363,7 @@
         <v>1.89E-3</v>
       </c>
     </row>
-    <row r="483" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A483" t="s">
         <v>494</v>
       </c>
@@ -19397,7 +19398,7 @@
         <v>2.99E-3</v>
       </c>
     </row>
-    <row r="484" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A484" t="s">
         <v>495</v>
       </c>
@@ -19432,7 +19433,7 @@
         <v>6.0800000000000003E-3</v>
       </c>
     </row>
-    <row r="485" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
         <v>496</v>
       </c>
@@ -19467,7 +19468,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="486" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A486" t="s">
         <v>497</v>
       </c>
@@ -19502,7 +19503,7 @@
         <v>2.8600000000000001E-3</v>
       </c>
     </row>
-    <row r="487" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
         <v>498</v>
       </c>
@@ -19537,7 +19538,7 @@
         <v>3.0599999999999998E-3</v>
       </c>
     </row>
-    <row r="488" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A488" t="s">
         <v>499</v>
       </c>
@@ -19572,7 +19573,7 @@
         <v>2.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="489" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A489" t="s">
         <v>500</v>
       </c>
@@ -19607,7 +19608,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="490" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A490" t="s">
         <v>501</v>
       </c>
@@ -19642,7 +19643,7 @@
         <v>4.9800000000000001E-3</v>
       </c>
     </row>
-    <row r="491" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A491" t="s">
         <v>502</v>
       </c>
@@ -19677,7 +19678,7 @@
         <v>3.8800000000000002E-3</v>
       </c>
     </row>
-    <row r="492" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
         <v>503</v>
       </c>
@@ -19712,7 +19713,7 @@
         <v>2.5400000000000002E-3</v>
       </c>
     </row>
-    <row r="493" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
         <v>504</v>
       </c>
@@ -19747,7 +19748,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="494" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
         <v>505</v>
       </c>
@@ -19782,7 +19783,7 @@
         <v>2.97E-3</v>
       </c>
     </row>
-    <row r="495" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
         <v>506</v>
       </c>
@@ -19817,7 +19818,7 @@
         <v>3.7200000000000002E-3</v>
       </c>
     </row>
-    <row r="496" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
         <v>507</v>
       </c>
@@ -19852,7 +19853,7 @@
         <v>3.8300000000000001E-3</v>
       </c>
     </row>
-    <row r="497" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>508</v>
       </c>
@@ -19887,7 +19888,7 @@
         <v>6.11E-3</v>
       </c>
     </row>
-    <row r="498" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
         <v>509</v>
       </c>
@@ -19922,7 +19923,7 @@
         <v>2.5400000000000002E-3</v>
       </c>
     </row>
-    <row r="499" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
         <v>510</v>
       </c>
@@ -19957,7 +19958,7 @@
         <v>2.3E-3</v>
       </c>
     </row>
-    <row r="500" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A500" t="s">
         <v>511</v>
       </c>
@@ -19992,7 +19993,7 @@
         <v>3.32E-3</v>
       </c>
     </row>
-    <row r="501" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
         <v>512</v>
       </c>
@@ -20027,7 +20028,7 @@
         <v>3.7100000000000002E-3</v>
       </c>
     </row>
-    <row r="502" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A502" t="s">
         <v>513</v>
       </c>
@@ -20062,7 +20063,7 @@
         <v>2.49E-3</v>
       </c>
     </row>
-    <row r="503" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
         <v>514</v>
       </c>
@@ -20097,7 +20098,7 @@
         <v>2.97E-3</v>
       </c>
     </row>
-    <row r="504" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
         <v>515</v>
       </c>
@@ -20132,7 +20133,7 @@
         <v>8.8400000000000006E-3</v>
       </c>
     </row>
-    <row r="505" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
         <v>516</v>
       </c>
@@ -20167,7 +20168,7 @@
         <v>4.3899999999999998E-3</v>
       </c>
     </row>
-    <row r="506" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A506" t="s">
         <v>517</v>
       </c>
@@ -20202,7 +20203,7 @@
         <v>6.0600000000000003E-3</v>
       </c>
     </row>
-    <row r="507" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
         <v>518</v>
       </c>
@@ -20237,7 +20238,7 @@
         <v>3.8500000000000001E-3</v>
       </c>
     </row>
-    <row r="508" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A508" t="s">
         <v>519</v>
       </c>
@@ -20272,7 +20273,7 @@
         <v>6.1399999999999996E-3</v>
       </c>
     </row>
-    <row r="509" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A509" t="s">
         <v>520</v>
       </c>
@@ -20307,7 +20308,7 @@
         <v>2.15E-3</v>
       </c>
     </row>
-    <row r="510" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A510" t="s">
         <v>521</v>
       </c>
@@ -20342,7 +20343,7 @@
         <v>2.5500000000000002E-3</v>
       </c>
     </row>
-    <row r="511" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
         <v>522</v>
       </c>
@@ -20377,7 +20378,7 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="512" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A512" t="s">
         <v>523</v>
       </c>
@@ -20412,7 +20413,7 @@
         <v>1.82E-3</v>
       </c>
     </row>
-    <row r="513" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
         <v>524</v>
       </c>
@@ -20447,7 +20448,7 @@
         <v>7.0800000000000004E-3</v>
       </c>
     </row>
-    <row r="514" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
         <v>525</v>
       </c>
@@ -20482,7 +20483,7 @@
         <v>4.7600000000000003E-3</v>
       </c>
     </row>
-    <row r="515" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A515" t="s">
         <v>526</v>
       </c>
@@ -20517,7 +20518,7 @@
         <v>5.0200000000000002E-3</v>
       </c>
     </row>
-    <row r="516" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A516" t="s">
         <v>527</v>
       </c>
@@ -20552,7 +20553,7 @@
         <v>6.5900000000000004E-3</v>
       </c>
     </row>
-    <row r="517" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A517" t="s">
         <v>528</v>
       </c>
@@ -20587,7 +20588,7 @@
         <v>4.0600000000000002E-3</v>
       </c>
     </row>
-    <row r="518" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A518" t="s">
         <v>529</v>
       </c>
@@ -20622,7 +20623,7 @@
         <v>3.0899999999999999E-3</v>
       </c>
     </row>
-    <row r="519" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A519" t="s">
         <v>530</v>
       </c>
@@ -20657,7 +20658,7 @@
         <v>2.7100000000000002E-3</v>
       </c>
     </row>
-    <row r="520" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A520" t="s">
         <v>531</v>
       </c>
@@ -20692,7 +20693,7 @@
         <v>4.1900000000000001E-3</v>
       </c>
     </row>
-    <row r="521" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A521" t="s">
         <v>532</v>
       </c>
@@ -20727,7 +20728,7 @@
         <v>5.6600000000000001E-3</v>
       </c>
     </row>
-    <row r="522" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A522" t="s">
         <v>533</v>
       </c>
@@ -20762,7 +20763,7 @@
         <v>7.26E-3</v>
       </c>
     </row>
-    <row r="523" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A523" t="s">
         <v>534</v>
       </c>
@@ -20797,7 +20798,7 @@
         <v>4.0899999999999999E-3</v>
       </c>
     </row>
-    <row r="524" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A524" t="s">
         <v>535</v>
       </c>
@@ -20832,7 +20833,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="525" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A525" t="s">
         <v>536</v>
       </c>
@@ -20867,7 +20868,7 @@
         <v>5.9300000000000004E-3</v>
       </c>
     </row>
-    <row r="526" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A526" t="s">
         <v>537</v>
       </c>
@@ -20902,7 +20903,7 @@
         <v>2.65E-3</v>
       </c>
     </row>
-    <row r="527" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A527" t="s">
         <v>538</v>
       </c>
@@ -20937,7 +20938,7 @@
         <v>2.2100000000000002E-3</v>
       </c>
     </row>
-    <row r="528" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A528" t="s">
         <v>539</v>
       </c>
@@ -20972,7 +20973,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="529" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A529" t="s">
         <v>540</v>
       </c>
@@ -21007,7 +21008,7 @@
         <v>7.0899999999999999E-3</v>
       </c>
     </row>
-    <row r="530" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A530" t="s">
         <v>541</v>
       </c>
@@ -21042,7 +21043,7 @@
         <v>3.2200000000000002E-3</v>
       </c>
     </row>
-    <row r="531" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A531" t="s">
         <v>542</v>
       </c>
@@ -21077,7 +21078,7 @@
         <v>3.6800000000000001E-3</v>
       </c>
     </row>
-    <row r="532" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A532" t="s">
         <v>543</v>
       </c>
@@ -21112,7 +21113,7 @@
         <v>4.6499999999999996E-3</v>
       </c>
     </row>
-    <row r="533" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A533" t="s">
         <v>544</v>
       </c>
@@ -21147,7 +21148,7 @@
         <v>2.7899999999999999E-3</v>
       </c>
     </row>
-    <row r="534" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A534" t="s">
         <v>545</v>
       </c>
@@ -21182,7 +21183,7 @@
         <v>2.5200000000000001E-3</v>
       </c>
     </row>
-    <row r="535" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A535" t="s">
         <v>546</v>
       </c>
@@ -21217,7 +21218,7 @@
         <v>3.5300000000000002E-3</v>
       </c>
     </row>
-    <row r="536" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A536" t="s">
         <v>547</v>
       </c>
@@ -21252,7 +21253,7 @@
         <v>6.2100000000000002E-3</v>
       </c>
     </row>
-    <row r="537" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A537" t="s">
         <v>548</v>
       </c>
@@ -21287,7 +21288,7 @@
         <v>2.32E-3</v>
       </c>
     </row>
-    <row r="538" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A538" t="s">
         <v>549</v>
       </c>
@@ -21322,7 +21323,7 @@
         <v>3.8700000000000002E-3</v>
       </c>
     </row>
-    <row r="539" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A539" t="s">
         <v>550</v>
       </c>
@@ -21357,7 +21358,7 @@
         <v>7.9600000000000001E-3</v>
       </c>
     </row>
-    <row r="540" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A540" t="s">
         <v>551</v>
       </c>
@@ -21392,7 +21393,7 @@
         <v>2.99E-3</v>
       </c>
     </row>
-    <row r="541" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A541" t="s">
         <v>552</v>
       </c>

</xml_diff>